<commit_message>
feat/fix(upload-data):adds search bar and fix update of data base
</commit_message>
<xml_diff>
--- a/follow_students/static/excel_format/FORMATO_SIS_CURSOS-NOTAS.xlsx
+++ b/follow_students/static/excel_format/FORMATO_SIS_CURSOS-NOTAS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Darwin Lenis\OneDrive\Escritorio\Universidad\5to Semestre\Proyecto Integrador\GitHub\Final-Project\follow_students\static\excel_format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F9E7FBB-5DF1-49C9-85BD-4B5DC059EF2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA3C799-8907-45F2-B5E9-6FA107BF9C4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{37C6A70E-0892-4DA6-B95F-1D86B2DF07FB}"/>
   </bookViews>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="6">
   <si>
     <t>Codigo</t>
   </si>
@@ -175,7 +175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -186,6 +186,9 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,7 +506,7 @@
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,7 +626,7 @@
         <v>1</v>
       </c>
       <c r="B19" s="2">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="4"/>
@@ -649,7 +652,7 @@
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
-      <c r="C23" s="3"/>
+      <c r="C23" s="6"/>
       <c r="D23" s="4"/>
     </row>
     <row r="24" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -657,7 +660,7 @@
         <v>4</v>
       </c>
       <c r="B24" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="4"/>
@@ -1133,8 +1136,8 @@
       <c r="A23" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>3</v>
+      <c r="B23" s="2">
+        <v>4.5</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="4"/>
@@ -1467,55 +1470,55 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83378612-03B1-4471-A6EF-74775669DB40}">
-  <dimension ref="A1:B38"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+  <dimension ref="A1:E38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O5" sqref="O5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
@@ -1523,23 +1526,23 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="2"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>1</v>
       </c>
@@ -1547,9 +1550,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
+      <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>

</xml_diff>

<commit_message>
fix(upload-data): fixs Nota _str_ in models
</commit_message>
<xml_diff>
--- a/follow_students/static/excel_format/FORMATO_SIS_CURSOS-NOTAS.xlsx
+++ b/follow_students/static/excel_format/FORMATO_SIS_CURSOS-NOTAS.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Darwin Lenis\OneDrive\Escritorio\Universidad\5to Semestre\Proyecto Integrador\GitHub\Final-Project\follow_students\static\excel_format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA3C799-8907-45F2-B5E9-6FA107BF9C4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A44D89-5DD1-40F9-9DF1-20E6A578B3A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{37C6A70E-0892-4DA6-B95F-1D86B2DF07FB}"/>
   </bookViews>
   <sheets>
-    <sheet name="_x0009_MAT-08273" sheetId="2" r:id="rId1"/>
+    <sheet name="MAT-08273" sheetId="2" r:id="rId1"/>
     <sheet name="ESJ-10094" sheetId="1" r:id="rId2"/>
     <sheet name="LEN-16001" sheetId="3" r:id="rId3"/>
     <sheet name="GES-01302" sheetId="4" r:id="rId4"/>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="7">
   <si>
     <t>Codigo</t>
   </si>
@@ -108,6 +108,9 @@
   </si>
   <si>
     <t>3.5</t>
+  </si>
+  <si>
+    <t>A00382021</t>
   </si>
 </sst>
 </file>
@@ -505,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7610B327-885F-4AAB-9C7A-CE572AFDF5EC}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,8 +647,12 @@
       <c r="D21" s="4"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="2"/>
+      <c r="A22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="2">
+        <v>1.2</v>
+      </c>
       <c r="C22" s="3"/>
       <c r="D22" s="4"/>
     </row>
@@ -989,7 +996,7 @@
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
chore(upload-data): changes xlsx format
</commit_message>
<xml_diff>
--- a/follow_students/static/excel_format/FORMATO_SIS_CURSOS-NOTAS.xlsx
+++ b/follow_students/static/excel_format/FORMATO_SIS_CURSOS-NOTAS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Darwin Lenis\OneDrive\Escritorio\Universidad\5to Semestre\Proyecto Integrador\GitHub\Final-Project\follow_students\static\excel_format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A44D89-5DD1-40F9-9DF1-20E6A578B3A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA201BB-F0B7-4EF5-97CA-8DB0522CB007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{37C6A70E-0892-4DA6-B95F-1D86B2DF07FB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{37C6A70E-0892-4DA6-B95F-1D86B2DF07FB}"/>
   </bookViews>
   <sheets>
     <sheet name="MAT-08273" sheetId="2" r:id="rId1"/>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="8">
   <si>
     <t>Codigo</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>A00382021</t>
+  </si>
+  <si>
+    <t>A00405266</t>
   </si>
 </sst>
 </file>
@@ -508,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7610B327-885F-4AAB-9C7A-CE572AFDF5EC}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,8 +610,12 @@
       <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="2"/>
+      <c r="A16" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1.2</v>
+      </c>
       <c r="C16" s="3"/>
       <c r="D16" s="4"/>
     </row>
@@ -996,7 +1003,7 @@
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1058,8 +1065,12 @@
       <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2"/>
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1.2</v>
+      </c>
       <c r="C10" s="3"/>
       <c r="D10" s="4"/>
     </row>
@@ -1480,7 +1491,7 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+      <selection activeCell="A19" sqref="A19:B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1571,8 +1582,12 @@
       <c r="B18" s="2"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="2"/>
+      <c r="A19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1.2</v>
+      </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
@@ -1890,7 +1905,7 @@
   <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2290,8 +2305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BC0D675-689C-40E4-9F18-21B34AF44FDB}">
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2417,8 +2432,12 @@
       <c r="B27" s="2"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="2"/>
+      <c r="A28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="2">
+        <v>1.2</v>
+      </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>

</xml_diff>

<commit_message>
style: translates upload data program director code
</commit_message>
<xml_diff>
--- a/follow_students/static/excel_format/FORMATO_SIS_CURSOS-NOTAS.xlsx
+++ b/follow_students/static/excel_format/FORMATO_SIS_CURSOS-NOTAS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Darwin Lenis\OneDrive\Escritorio\Universidad\5to Semestre\Proyecto Integrador\GitHub\Final-Project\follow_students\static\excel_format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EA201BB-F0B7-4EF5-97CA-8DB0522CB007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF9639EE-59A9-47BA-986F-3048102D2D38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{37C6A70E-0892-4DA6-B95F-1D86B2DF07FB}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11295" activeTab="5" xr2:uid="{37C6A70E-0892-4DA6-B95F-1D86B2DF07FB}"/>
   </bookViews>
   <sheets>
     <sheet name="MAT-08273" sheetId="2" r:id="rId1"/>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="8">
   <si>
     <t>Codigo</t>
   </si>
@@ -2305,8 +2305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BC0D675-689C-40E4-9F18-21B34AF44FDB}">
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28:B28"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2626,77 +2626,82 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74C0C75F-C9B6-4BCF-ABB9-B7B70F863CE0}">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B38"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="2">
+        <v>5</v>
+      </c>
+      <c r="C12" s="5"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="2"/>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
     </row>

</xml_diff>

<commit_message>
refactor: adds name of courses
</commit_message>
<xml_diff>
--- a/follow_students/static/excel_format/FORMATO_SIS_CURSOS-NOTAS.xlsx
+++ b/follow_students/static/excel_format/FORMATO_SIS_CURSOS-NOTAS.xlsx
@@ -8,26 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Darwin Lenis\OneDrive\Escritorio\Universidad\5to Semestre\Proyecto Integrador\GitHub\Final-Project\follow_students\static\excel_format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF9639EE-59A9-47BA-986F-3048102D2D38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02CCE75D-C7CE-4728-896B-B60423366E9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11295" activeTab="5" xr2:uid="{37C6A70E-0892-4DA6-B95F-1D86B2DF07FB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="11" activeTab="14" xr2:uid="{37C6A70E-0892-4DA6-B95F-1D86B2DF07FB}"/>
   </bookViews>
   <sheets>
-    <sheet name="MAT-08273" sheetId="2" r:id="rId1"/>
-    <sheet name="ESJ-10094" sheetId="1" r:id="rId2"/>
-    <sheet name="LEN-16001" sheetId="3" r:id="rId3"/>
-    <sheet name="GES-01302" sheetId="4" r:id="rId4"/>
-    <sheet name="TIC-09777" sheetId="6" r:id="rId5"/>
-    <sheet name="MAT-08272" sheetId="7" r:id="rId6"/>
-    <sheet name="TIC-09703" sheetId="45" r:id="rId7"/>
-    <sheet name="LEN-16002" sheetId="44" r:id="rId8"/>
-    <sheet name="TIC-09782" sheetId="46" r:id="rId9"/>
-    <sheet name="CFT-11354" sheetId="47" r:id="rId10"/>
-    <sheet name="HUM-06221" sheetId="49" r:id="rId11"/>
-    <sheet name="TIC-09704" sheetId="51" r:id="rId12"/>
-    <sheet name="TIC-09781" sheetId="52" r:id="rId13"/>
-    <sheet name="TIC-09773" sheetId="53" r:id="rId14"/>
-    <sheet name="HUM-02222" sheetId="54" r:id="rId15"/>
+    <sheet name="MAT-08273_Logica" sheetId="2" r:id="rId1"/>
+    <sheet name="ESJ-10094_FundamentosDerecho" sheetId="1" r:id="rId2"/>
+    <sheet name="LEN-16001_COE1" sheetId="3" r:id="rId3"/>
+    <sheet name="GES-01302_Organizaciones" sheetId="4" r:id="rId4"/>
+    <sheet name="TIC-09777_IntroSIS" sheetId="6" r:id="rId5"/>
+    <sheet name="MAT-08272_Algebra y funciones" sheetId="7" r:id="rId6"/>
+    <sheet name="TIC-09703_APO" sheetId="45" r:id="rId7"/>
+    <sheet name="LEN-16002_COE2" sheetId="44" r:id="rId8"/>
+    <sheet name="TIC-09782_Inge Soft 1" sheetId="46" r:id="rId9"/>
+    <sheet name="CFT-11354_Mat Aplicadas 1" sheetId="47" r:id="rId10"/>
+    <sheet name="HUM-06221_Principios Economia" sheetId="49" r:id="rId11"/>
+    <sheet name="TIC-09704_APO2" sheetId="51" r:id="rId12"/>
+    <sheet name="TIC-09781_Discretas 1" sheetId="52" r:id="rId13"/>
+    <sheet name="TIC-09773_Inge Soft 2" sheetId="53" r:id="rId14"/>
+    <sheet name="HUM-02222_Electiva" sheetId="54" r:id="rId15"/>
     <sheet name="CFT-08310" sheetId="55" r:id="rId16"/>
     <sheet name="MAT-08131" sheetId="56" r:id="rId17"/>
     <sheet name="TIC-09768" sheetId="58" r:id="rId18"/>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="8">
   <si>
     <t>Codigo</t>
   </si>
@@ -181,7 +181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -195,6 +195,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -509,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7610B327-885F-4AAB-9C7A-CE572AFDF5EC}">
-  <dimension ref="A1:D38"/>
-  <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:B16"/>
+  <dimension ref="A1:J38"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,6 +620,504 @@
       <c r="C16" s="3"/>
       <c r="D16" s="4"/>
     </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1</v>
+      </c>
+      <c r="C24" s="3"/>
+      <c r="D24" s="4"/>
+      <c r="F24" s="5"/>
+      <c r="J24" s="5"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="4"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="4"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="5"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="4"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="4"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="4"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="4"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="4"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="4"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D5E492E-6C95-4C56-8BE5-A7ACE9CE2759}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{555CC038-3FF4-4B23-A920-B9AC60599B2F}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{248DCCBE-138F-4566-B8B0-B09077A7DAB5}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCC6CC24-F21C-4136-94F5-AAC5A980B15C}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42DBC65C-CF1A-4866-A68B-CC1C0EE19CDB}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D5AC12-E59D-4EC3-A3CB-451A4D0B17BE}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92F8DEBF-4280-4009-9629-C2C8221475F6}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B145DD2B-C47A-4E24-A8C2-9F938BBED345}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3E8FA73-9F48-4AD6-89EA-4166F6516606}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCAB00A3-EEA4-4B08-98EB-C11EEC1C0041}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF789E85-769D-4EA3-94AE-AA3E51CDE9C9}">
+  <dimension ref="A1:D38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="2">
+        <v>4</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="4"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="4"/>
+    </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
@@ -632,12 +1131,8 @@
       <c r="D18" s="4"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" s="2">
-        <v>4.5</v>
-      </c>
+      <c r="A19" s="1"/>
+      <c r="B19" s="2"/>
       <c r="C19" s="3"/>
       <c r="D19" s="4"/>
     </row>
@@ -654,28 +1149,24 @@
       <c r="D21" s="4"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="2">
-        <v>1.2</v>
-      </c>
+      <c r="A22" s="1"/>
+      <c r="B22" s="2"/>
       <c r="C22" s="3"/>
       <c r="D22" s="4"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="6"/>
+      <c r="A23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="C23" s="3"/>
       <c r="D23" s="4"/>
     </row>
-    <row r="24" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24" s="2">
-        <v>1</v>
-      </c>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="2"/>
       <c r="C24" s="3"/>
       <c r="D24" s="4"/>
     </row>
@@ -764,493 +1255,6 @@
       <c r="D38" s="4"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D5E492E-6C95-4C56-8BE5-A7ACE9CE2759}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{555CC038-3FF4-4B23-A920-B9AC60599B2F}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{248DCCBE-138F-4566-B8B0-B09077A7DAB5}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCC6CC24-F21C-4136-94F5-AAC5A980B15C}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42DBC65C-CF1A-4866-A68B-CC1C0EE19CDB}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D5AC12-E59D-4EC3-A3CB-451A4D0B17BE}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92F8DEBF-4280-4009-9629-C2C8221475F6}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B145DD2B-C47A-4E24-A8C2-9F938BBED345}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3E8FA73-9F48-4AD6-89EA-4166F6516606}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCAB00A3-EEA4-4B08-98EB-C11EEC1C0041}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF789E85-769D-4EA3-94AE-AA3E51CDE9C9}">
-  <dimension ref="A1:D38"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="2">
-        <v>4</v>
-      </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="4"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="4"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="4"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" s="2">
-        <v>4.5</v>
-      </c>
-      <c r="C23" s="3"/>
-      <c r="D23" s="4"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="4"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="4"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="4"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="4"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="4"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="4"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="4"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="4"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="4"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="4"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="4"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="4"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="4"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="2"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="4"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="4"/>
-    </row>
-  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2303,10 +2307,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BC0D675-689C-40E4-9F18-21B34AF44FDB}">
-  <dimension ref="A1:B38"/>
-  <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:B20"/>
+  <dimension ref="A1:N38"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2379,19 +2383,19 @@
       <c r="A16" s="1"/>
       <c r="B16" s="2"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="2"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="2"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>1</v>
       </c>
@@ -2399,19 +2403,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="2"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="N22" s="5"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="2"/>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>4</v>
       </c>
@@ -2419,19 +2424,19 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>7</v>
       </c>
@@ -2439,19 +2444,19 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
     </row>
@@ -2626,8 +2631,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74C0C75F-C9B6-4BCF-ABB9-B7B70F863CE0}">
   <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2801,21 +2806,175 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8329DD4F-962D-428A-8E6F-9E1B614ADE76}">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection sqref="A1:B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>2</v>
-      </c>
+  <dimension ref="A1:G38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="2">
+        <v>5</v>
+      </c>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="2"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="2"/>
+      <c r="G28" s="5"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="2"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="2"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="2"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="2"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="2"/>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="2"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+      <c r="B35" s="2"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="2"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="2"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+      <c r="B38" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>